<commit_message>
Updated 02.21.2021, ~11:30am CST
</commit_message>
<xml_diff>
--- a/Source Assignment.xlsx
+++ b/Source Assignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Math 5545 Project 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64e1b9c56e7ec9ea/Documents/UMKC/MATH 490/GP1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05B766B-61B9-4F8F-A771-F108B7568813}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{C05B766B-61B9-4F8F-A771-F108B7568813}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EA941425-AFFF-420B-B559-D0B331580CB0}"/>
   <bookViews>
-    <workbookView xWindow="10755" yWindow="2655" windowWidth="14895" windowHeight="11385" xr2:uid="{7C30F52E-DFEE-471B-868A-F17E658BCBA7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7C30F52E-DFEE-471B-868A-F17E658BCBA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>High</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t>KCEPS</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,78 +511,221 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2">
+        <v>4440</v>
+      </c>
+      <c r="C2">
+        <v>20468</v>
+      </c>
+      <c r="D2">
+        <v>5345</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B3">
+        <v>248</v>
+      </c>
+      <c r="C3">
+        <v>2307</v>
+      </c>
+      <c r="D3">
+        <v>1471</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B4">
+        <v>1030</v>
+      </c>
+      <c r="C4">
+        <v>8929</v>
+      </c>
+      <c r="D4">
+        <v>3438</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B5">
+        <v>85</v>
+      </c>
+      <c r="C5">
+        <v>155</v>
+      </c>
+      <c r="D5">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>410</v>
+      </c>
+      <c r="D6">
+        <v>139</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B8">
+        <v>341</v>
+      </c>
+      <c r="C8">
+        <v>2441</v>
+      </c>
+      <c r="D8">
+        <v>1025</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>